<commit_message>
Add optional Learners Profile feature to auto-fill LRN, Birthday, and Sex
- Add optional learners profile upload in web interface
- Auto-fill LRN (Row 10, Col J), Birthday (Row 10, Col U), Sex (Row 10, Col AS)
- Implement name normalization to handle comma spacing variations
- If no profile uploaded, fields remain blank
- Update UI: add Section 2 for Learners Profile with drag-and-drop
- Clean SF10 template by removing hardcoded sample data
- Update terminology from 'Gender' to 'Sex' to match SF10 form
</commit_message>
<xml_diff>
--- a/assets/docs/SF10.xlsx
+++ b/assets/docs/SF10.xlsx
@@ -2051,6 +2051,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2076,6 +2079,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -2457,7 +2463,7 @@
     <col width="4.7109375" customWidth="1" style="2" min="48" max="48"/>
     <col width="7.42578125" customWidth="1" style="2" min="49" max="49"/>
     <col width="0.7109375" customWidth="1" style="2" min="50" max="50"/>
-    <col hidden="1" style="2" min="51" max="52"/>
+    <col hidden="1" width="13" customWidth="1" style="2" min="51" max="52"/>
     <col hidden="1" width="9.28515625" customWidth="1" style="2" min="53" max="16384"/>
   </cols>
   <sheetData>
@@ -2784,11 +2790,7 @@
           <t>LAST NAME:</t>
         </is>
       </c>
-      <c r="E9" s="205" t="inlineStr">
-        <is>
-          <t>AGOT</t>
-        </is>
-      </c>
+      <c r="E9" s="205" t="inlineStr"/>
       <c r="F9" s="214" t="n"/>
       <c r="G9" s="214" t="n"/>
       <c r="H9" s="214" t="n"/>
@@ -2801,11 +2803,7 @@
           <t>FIRST NAME:</t>
         </is>
       </c>
-      <c r="Q9" s="206" t="inlineStr">
-        <is>
-          <t>KHIAN CLOUD</t>
-        </is>
-      </c>
+      <c r="Q9" s="206" t="inlineStr"/>
       <c r="R9" s="212" t="n"/>
       <c r="S9" s="212" t="n"/>
       <c r="T9" s="212" t="n"/>
@@ -2837,11 +2835,7 @@
       <c r="AL9" s="8" t="n"/>
       <c r="AM9" s="8" t="n"/>
       <c r="AN9" s="8" t="n"/>
-      <c r="AP9" s="205" t="inlineStr">
-        <is>
-          <t>DABLO</t>
-        </is>
-      </c>
+      <c r="AP9" s="205" t="inlineStr"/>
       <c r="AQ9" s="214" t="n"/>
       <c r="AR9" s="214" t="n"/>
       <c r="AS9" s="214" t="n"/>
@@ -2864,9 +2858,7 @@
       <c r="G10" s="7" t="n"/>
       <c r="H10" s="7" t="n"/>
       <c r="I10" s="7" t="n"/>
-      <c r="J10" s="189" t="n">
-        <v>162508230415</v>
-      </c>
+      <c r="J10" s="189" t="inlineStr"/>
       <c r="K10" s="215" t="n"/>
       <c r="L10" s="215" t="n"/>
       <c r="M10" s="215" t="n"/>
@@ -2876,9 +2868,7 @@
           <t>Birthdate (mm/dd/yyyy):</t>
         </is>
       </c>
-      <c r="U10" s="190" t="n">
-        <v>43071</v>
-      </c>
+      <c r="U10" s="190" t="inlineStr"/>
       <c r="V10" s="215" t="n"/>
       <c r="W10" s="215" t="n"/>
       <c r="X10" s="215" t="n"/>
@@ -2899,11 +2889,7 @@
           <t xml:space="preserve">Sex: </t>
         </is>
       </c>
-      <c r="AS10" s="191" t="inlineStr">
-        <is>
-          <t>MALE</t>
-        </is>
-      </c>
+      <c r="AS10" s="191" t="inlineStr"/>
       <c r="AT10" s="215" t="n"/>
       <c r="AU10" s="215" t="n"/>
       <c r="AV10" s="215" t="n"/>
@@ -4010,18 +3996,10 @@
       <c r="H30" s="212" t="n"/>
       <c r="I30" s="212" t="n"/>
       <c r="J30" s="213" t="n"/>
-      <c r="K30" s="48" t="n">
-        <v>83</v>
-      </c>
-      <c r="L30" s="48" t="n">
-        <v>81</v>
-      </c>
-      <c r="M30" s="48" t="n">
-        <v>82</v>
-      </c>
-      <c r="N30" s="48" t="n">
-        <v>82</v>
-      </c>
+      <c r="K30" s="48" t="inlineStr"/>
+      <c r="L30" s="48" t="inlineStr"/>
+      <c r="M30" s="48" t="inlineStr"/>
+      <c r="N30" s="48" t="inlineStr"/>
       <c r="O30" s="243">
         <f>AVERAGE(K30:N30)</f>
         <v/>
@@ -4081,18 +4059,10 @@
       <c r="H31" s="212" t="n"/>
       <c r="I31" s="212" t="n"/>
       <c r="J31" s="213" t="n"/>
-      <c r="K31" s="48" t="n">
-        <v>81</v>
-      </c>
-      <c r="L31" s="48" t="n">
-        <v>80</v>
-      </c>
-      <c r="M31" s="48" t="n">
-        <v>81</v>
-      </c>
-      <c r="N31" s="48" t="n">
-        <v>81</v>
-      </c>
+      <c r="K31" s="48" t="inlineStr"/>
+      <c r="L31" s="48" t="inlineStr"/>
+      <c r="M31" s="48" t="inlineStr"/>
+      <c r="N31" s="48" t="inlineStr"/>
       <c r="O31" s="243">
         <f>AVERAGE(K31:N31)</f>
         <v/>
@@ -4152,18 +4122,10 @@
       <c r="H32" s="212" t="n"/>
       <c r="I32" s="212" t="n"/>
       <c r="J32" s="213" t="n"/>
-      <c r="K32" s="48" t="n">
-        <v>86</v>
-      </c>
-      <c r="L32" s="48" t="n">
-        <v>85</v>
-      </c>
-      <c r="M32" s="51" t="n">
-        <v>86</v>
-      </c>
-      <c r="N32" s="48" t="n">
-        <v>86</v>
-      </c>
+      <c r="K32" s="48" t="inlineStr"/>
+      <c r="L32" s="48" t="inlineStr"/>
+      <c r="M32" s="51" t="inlineStr"/>
+      <c r="N32" s="48" t="inlineStr"/>
       <c r="O32" s="243">
         <f>AVERAGE(K32:N32)</f>
         <v/>
@@ -4223,18 +4185,10 @@
       <c r="H33" s="212" t="n"/>
       <c r="I33" s="212" t="n"/>
       <c r="J33" s="213" t="n"/>
-      <c r="K33" s="48" t="n">
-        <v>85</v>
-      </c>
-      <c r="L33" s="52" t="n">
-        <v>85</v>
-      </c>
-      <c r="M33" s="52" t="n">
-        <v>86</v>
-      </c>
-      <c r="N33" s="48" t="n">
-        <v>87</v>
-      </c>
+      <c r="K33" s="48" t="inlineStr"/>
+      <c r="L33" s="52" t="inlineStr"/>
+      <c r="M33" s="52" t="inlineStr"/>
+      <c r="N33" s="48" t="inlineStr"/>
       <c r="O33" s="243">
         <f>AVERAGE(K33:N33)</f>
         <v/>
@@ -4294,18 +4248,10 @@
       <c r="H34" s="212" t="n"/>
       <c r="I34" s="212" t="n"/>
       <c r="J34" s="213" t="n"/>
-      <c r="K34" s="48" t="n">
-        <v>85</v>
-      </c>
-      <c r="L34" s="48" t="n">
-        <v>84</v>
-      </c>
-      <c r="M34" s="51" t="n">
-        <v>85</v>
-      </c>
-      <c r="N34" s="52" t="n">
-        <v>86</v>
-      </c>
+      <c r="K34" s="48" t="inlineStr"/>
+      <c r="L34" s="48" t="inlineStr"/>
+      <c r="M34" s="51" t="inlineStr"/>
+      <c r="N34" s="52" t="inlineStr"/>
       <c r="O34" s="243">
         <f>AVERAGE(K34:N34)</f>
         <v/>

</xml_diff>